<commit_message>
Closed init file after reading init data. Annuity payment changed to month because of annuity coef problem
</commit_message>
<xml_diff>
--- a/LabWork1/init data.xlsx
+++ b/LabWork1/init data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skiv2\OneDrive\Documents\GitHub\JavaEduNSU\LabWork1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user2\source\repos\JavaEduNSU\JavaEduNSU\LabWork1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEED6C13-D781-4D63-A5EA-D1B30AC885E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9407A6FC-E97E-4FFA-ACCC-45D572033B82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{C951D278-9AB7-494D-8ADB-E95B64F142C0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C951D278-9AB7-494D-8ADB-E95B64F142C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>